<commit_message>
modified the report plugin
</commit_message>
<xml_diff>
--- a/src/test/resources/config/contactusData.xlsx
+++ b/src/test/resources/config/contactusData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rames\eclipse-workspace\CucumberWizards\src\test\resources\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OldLaptop\Selenium\CucumberWizards\src\test\resources\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44394D15-F086-4AA5-B580-0B72726851D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC930FA-4C35-4FC2-B4A4-438228032B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3000" windowWidth="17280" windowHeight="8880" xr2:uid="{11AC1E02-68E5-41D6-B65F-0A14C381B0C2}"/>
+    <workbookView xWindow="4392" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{11AC1E02-68E5-41D6-B65F-0A14C381B0C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Contactus" sheetId="1" r:id="rId1"/>
@@ -429,7 +429,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>